<commit_message>
Need to do Logs
</commit_message>
<xml_diff>
--- a/ref/DataSheet.xlsx
+++ b/ref/DataSheet.xlsx
@@ -286,7 +286,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -380,15 +380,99 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="90"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="174"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="90" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="174" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -401,7 +485,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="90"/>
+    <cellStyle name="Hyperlink" xfId="174"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>

</xml_diff>